<commit_message>
Working version of bot
</commit_message>
<xml_diff>
--- a/SeminarDatasheet.xlsx
+++ b/SeminarDatasheet.xlsx
@@ -1,25 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\usersp\gjunyujo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Stuff\Development\Python\excel-bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E0FBE6-4381-4997-825C-4AF6A4861ADC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9600"/>
+    <workbookView xWindow="8445" yWindow="3000" windowWidth="14400" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -35,28 +31,28 @@
     <t>REGISTER</t>
   </si>
   <si>
+    <t>5148A</t>
+  </si>
+  <si>
     <t>A</t>
   </si>
   <si>
+    <t>7713Z</t>
+  </si>
+  <si>
     <t>B</t>
   </si>
   <si>
+    <t>1543H</t>
+  </si>
+  <si>
     <t>C</t>
   </si>
   <si>
+    <t>1935B</t>
+  </si>
+  <si>
     <t>D</t>
-  </si>
-  <si>
-    <t>5148A</t>
-  </si>
-  <si>
-    <t>7713Z</t>
-  </si>
-  <si>
-    <t>1543H</t>
-  </si>
-  <si>
-    <t>1935B</t>
   </si>
   <si>
     <t>5337J</t>
@@ -1247,7 +1243,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1587,19 +1583,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D400"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="2"/>
-    <col min="5" max="16384" width="9.140625" style="2"/>
+    <col min="3" max="3" width="9.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1615,37 +1613,37 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1"/>
     </row>
@@ -1654,7 +1652,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -1663,7 +1661,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -1672,7 +1670,7 @@
         <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C8" s="1"/>
     </row>
@@ -1681,7 +1679,7 @@
         <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C9" s="1"/>
     </row>
@@ -1690,7 +1688,7 @@
         <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C10" s="1"/>
     </row>
@@ -1699,7 +1697,7 @@
         <v>16</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C11" s="1"/>
     </row>
@@ -1708,7 +1706,7 @@
         <v>17</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C12" s="1"/>
     </row>
@@ -1717,7 +1715,7 @@
         <v>18</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C13" s="1"/>
     </row>
@@ -1726,7 +1724,7 @@
         <v>19</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C14" s="1"/>
     </row>
@@ -1735,7 +1733,7 @@
         <v>20</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C15" s="1"/>
     </row>
@@ -1744,7 +1742,7 @@
         <v>21</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C16" s="1"/>
     </row>
@@ -1753,7 +1751,7 @@
         <v>22</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C17" s="1"/>
     </row>
@@ -1762,7 +1760,7 @@
         <v>23</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C18" s="1"/>
     </row>
@@ -1771,7 +1769,7 @@
         <v>24</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C19" s="1"/>
     </row>
@@ -1780,7 +1778,7 @@
         <v>25</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C20" s="1"/>
     </row>
@@ -1789,7 +1787,7 @@
         <v>26</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C21" s="1"/>
     </row>
@@ -1798,7 +1796,7 @@
         <v>27</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C22" s="1"/>
     </row>
@@ -1807,7 +1805,7 @@
         <v>28</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C23" s="1"/>
     </row>
@@ -1816,7 +1814,7 @@
         <v>29</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C24" s="1"/>
     </row>
@@ -1825,7 +1823,7 @@
         <v>30</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C25" s="1"/>
     </row>
@@ -1834,7 +1832,7 @@
         <v>31</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C26" s="1"/>
     </row>
@@ -1843,7 +1841,7 @@
         <v>32</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C27" s="1"/>
     </row>
@@ -1852,7 +1850,7 @@
         <v>33</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C28" s="1"/>
     </row>
@@ -1861,7 +1859,7 @@
         <v>34</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C29" s="1"/>
     </row>
@@ -1870,7 +1868,7 @@
         <v>35</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C30" s="1"/>
     </row>
@@ -1879,7 +1877,7 @@
         <v>36</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C31" s="1"/>
     </row>
@@ -1888,7 +1886,7 @@
         <v>37</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C32" s="1"/>
     </row>
@@ -1897,7 +1895,7 @@
         <v>38</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C33" s="1"/>
     </row>
@@ -1906,7 +1904,7 @@
         <v>39</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C34" s="1"/>
     </row>
@@ -1915,7 +1913,7 @@
         <v>40</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C35" s="1"/>
     </row>
@@ -1924,7 +1922,7 @@
         <v>41</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C36" s="1"/>
     </row>
@@ -1933,7 +1931,7 @@
         <v>42</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C37" s="1"/>
     </row>
@@ -1942,7 +1940,7 @@
         <v>43</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C38" s="1"/>
     </row>
@@ -1951,7 +1949,7 @@
         <v>44</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C39" s="1"/>
     </row>
@@ -1960,7 +1958,7 @@
         <v>45</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C40" s="1"/>
     </row>
@@ -1969,7 +1967,7 @@
         <v>46</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C41" s="1"/>
     </row>
@@ -1978,7 +1976,7 @@
         <v>47</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C42" s="1"/>
     </row>
@@ -1987,7 +1985,7 @@
         <v>48</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C43" s="1"/>
     </row>
@@ -1996,7 +1994,7 @@
         <v>49</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C44" s="1"/>
     </row>
@@ -2005,7 +2003,7 @@
         <v>50</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C45" s="1"/>
     </row>
@@ -2014,7 +2012,7 @@
         <v>51</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C46" s="1"/>
     </row>
@@ -2023,7 +2021,7 @@
         <v>52</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C47" s="1"/>
     </row>
@@ -2032,7 +2030,7 @@
         <v>53</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C48" s="1"/>
     </row>
@@ -2041,7 +2039,7 @@
         <v>54</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C49" s="1"/>
     </row>
@@ -2050,7 +2048,7 @@
         <v>55</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C50" s="1"/>
     </row>
@@ -2059,7 +2057,7 @@
         <v>56</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C51" s="1"/>
     </row>
@@ -2068,7 +2066,7 @@
         <v>57</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C52" s="1"/>
     </row>
@@ -2077,7 +2075,7 @@
         <v>58</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C53" s="1"/>
     </row>
@@ -2086,7 +2084,7 @@
         <v>59</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C54" s="1"/>
     </row>
@@ -2095,7 +2093,7 @@
         <v>60</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C55" s="1"/>
     </row>
@@ -2104,7 +2102,7 @@
         <v>61</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C56" s="1"/>
     </row>
@@ -2113,7 +2111,7 @@
         <v>62</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C57" s="1"/>
     </row>
@@ -2122,7 +2120,7 @@
         <v>63</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C58" s="1"/>
     </row>
@@ -2131,7 +2129,7 @@
         <v>64</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C59" s="1"/>
     </row>
@@ -2140,7 +2138,7 @@
         <v>65</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C60" s="1"/>
     </row>
@@ -2149,7 +2147,7 @@
         <v>66</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C61" s="1"/>
     </row>
@@ -2158,7 +2156,7 @@
         <v>67</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C62" s="1"/>
     </row>
@@ -2167,7 +2165,7 @@
         <v>68</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C63" s="1"/>
     </row>
@@ -2176,7 +2174,7 @@
         <v>69</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C64" s="1"/>
     </row>
@@ -2185,7 +2183,7 @@
         <v>70</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C65" s="1"/>
     </row>
@@ -2194,7 +2192,7 @@
         <v>71</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C66" s="1"/>
     </row>
@@ -2203,7 +2201,7 @@
         <v>72</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C67" s="1"/>
     </row>
@@ -2212,7 +2210,7 @@
         <v>73</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C68" s="1"/>
     </row>
@@ -2221,7 +2219,7 @@
         <v>74</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C69" s="1"/>
     </row>
@@ -2230,7 +2228,7 @@
         <v>75</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C70" s="1"/>
     </row>
@@ -2239,7 +2237,7 @@
         <v>76</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C71" s="1"/>
     </row>
@@ -2248,7 +2246,7 @@
         <v>77</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C72" s="1"/>
     </row>
@@ -2257,7 +2255,7 @@
         <v>78</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C73" s="1"/>
     </row>
@@ -2266,7 +2264,7 @@
         <v>79</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C74" s="1"/>
     </row>
@@ -2275,7 +2273,7 @@
         <v>80</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C75" s="1"/>
     </row>
@@ -2284,7 +2282,7 @@
         <v>81</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C76" s="1"/>
     </row>
@@ -2293,7 +2291,7 @@
         <v>82</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C77" s="1"/>
     </row>
@@ -2302,7 +2300,7 @@
         <v>83</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C78" s="1"/>
     </row>
@@ -2311,7 +2309,7 @@
         <v>84</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C79" s="1"/>
     </row>
@@ -2320,7 +2318,7 @@
         <v>85</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C80" s="1"/>
     </row>
@@ -2329,7 +2327,7 @@
         <v>86</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C81" s="1"/>
     </row>
@@ -2338,7 +2336,7 @@
         <v>87</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C82" s="1"/>
     </row>
@@ -2347,7 +2345,7 @@
         <v>88</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C83" s="1"/>
     </row>
@@ -2356,7 +2354,7 @@
         <v>89</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C84" s="1"/>
     </row>
@@ -2365,7 +2363,7 @@
         <v>90</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C85" s="1"/>
     </row>
@@ -2374,7 +2372,7 @@
         <v>91</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C86" s="1"/>
     </row>
@@ -2383,7 +2381,7 @@
         <v>92</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C87" s="1"/>
     </row>
@@ -2392,7 +2390,7 @@
         <v>93</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C88" s="1"/>
     </row>
@@ -2401,7 +2399,7 @@
         <v>94</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C89" s="1"/>
     </row>
@@ -2410,7 +2408,7 @@
         <v>95</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C90" s="1"/>
     </row>
@@ -2419,7 +2417,7 @@
         <v>96</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C91" s="1"/>
     </row>
@@ -2428,7 +2426,7 @@
         <v>97</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C92" s="1"/>
     </row>
@@ -2437,7 +2435,7 @@
         <v>98</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C93" s="1"/>
     </row>
@@ -2446,7 +2444,7 @@
         <v>99</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C94" s="1"/>
     </row>
@@ -2455,7 +2453,7 @@
         <v>100</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C95" s="1"/>
     </row>
@@ -2464,7 +2462,7 @@
         <v>101</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C96" s="1"/>
     </row>
@@ -2473,7 +2471,7 @@
         <v>102</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C97" s="1"/>
     </row>
@@ -2482,7 +2480,7 @@
         <v>103</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C98" s="1"/>
     </row>
@@ -2491,7 +2489,7 @@
         <v>104</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C99" s="1"/>
     </row>
@@ -2500,7 +2498,7 @@
         <v>105</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C100" s="1"/>
     </row>
@@ -2509,7 +2507,7 @@
         <v>106</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C101" s="1"/>
     </row>
@@ -2518,7 +2516,7 @@
         <v>107</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C102" s="1"/>
     </row>
@@ -2527,7 +2525,7 @@
         <v>108</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C103" s="1"/>
     </row>
@@ -2536,7 +2534,7 @@
         <v>109</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C104" s="1"/>
     </row>
@@ -2545,7 +2543,7 @@
         <v>110</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C105" s="1"/>
     </row>
@@ -2554,7 +2552,7 @@
         <v>111</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C106" s="1"/>
     </row>
@@ -2563,7 +2561,7 @@
         <v>112</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C107" s="1"/>
     </row>
@@ -2572,7 +2570,7 @@
         <v>113</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C108" s="1"/>
     </row>
@@ -2581,7 +2579,7 @@
         <v>114</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C109" s="1"/>
     </row>
@@ -2590,7 +2588,7 @@
         <v>115</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C110" s="1"/>
     </row>
@@ -2599,7 +2597,7 @@
         <v>116</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C111" s="1"/>
     </row>
@@ -2608,7 +2606,7 @@
         <v>117</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C112" s="1"/>
     </row>
@@ -2617,7 +2615,7 @@
         <v>118</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C113" s="1"/>
     </row>
@@ -2626,7 +2624,7 @@
         <v>119</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C114" s="1"/>
     </row>
@@ -2635,7 +2633,7 @@
         <v>120</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C115" s="1"/>
     </row>
@@ -2644,7 +2642,7 @@
         <v>121</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C116" s="1"/>
     </row>
@@ -2653,7 +2651,7 @@
         <v>122</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C117" s="1"/>
     </row>
@@ -2662,7 +2660,7 @@
         <v>123</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C118" s="1"/>
     </row>
@@ -2671,7 +2669,7 @@
         <v>124</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C119" s="1"/>
     </row>
@@ -2680,7 +2678,7 @@
         <v>125</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C120" s="1"/>
     </row>
@@ -2689,7 +2687,7 @@
         <v>126</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C121" s="1"/>
     </row>
@@ -2698,7 +2696,7 @@
         <v>127</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C122" s="1"/>
     </row>
@@ -2707,7 +2705,7 @@
         <v>128</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C123" s="1"/>
     </row>
@@ -2716,7 +2714,7 @@
         <v>129</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C124" s="1"/>
     </row>
@@ -2725,7 +2723,7 @@
         <v>130</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C125" s="1"/>
     </row>
@@ -2734,7 +2732,7 @@
         <v>131</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C126" s="1"/>
     </row>
@@ -2743,7 +2741,7 @@
         <v>132</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C127" s="1"/>
     </row>
@@ -2752,7 +2750,7 @@
         <v>133</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C128" s="1"/>
     </row>
@@ -2761,7 +2759,7 @@
         <v>134</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C129" s="1"/>
     </row>
@@ -2770,7 +2768,7 @@
         <v>135</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C130" s="1"/>
     </row>
@@ -2779,7 +2777,7 @@
         <v>136</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C131" s="1"/>
     </row>
@@ -2788,7 +2786,7 @@
         <v>137</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C132" s="1"/>
     </row>
@@ -2797,7 +2795,7 @@
         <v>138</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C133" s="1"/>
     </row>
@@ -2806,7 +2804,7 @@
         <v>139</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C134" s="1"/>
     </row>
@@ -2815,7 +2813,7 @@
         <v>140</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C135" s="1"/>
     </row>
@@ -2824,7 +2822,7 @@
         <v>141</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C136" s="1"/>
     </row>
@@ -2833,7 +2831,7 @@
         <v>142</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C137" s="1"/>
     </row>
@@ -2842,7 +2840,7 @@
         <v>143</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C138" s="1"/>
     </row>
@@ -2851,7 +2849,7 @@
         <v>144</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C139" s="1"/>
     </row>
@@ -2860,7 +2858,7 @@
         <v>145</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C140" s="1"/>
     </row>
@@ -2869,7 +2867,7 @@
         <v>146</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C141" s="1"/>
     </row>
@@ -2878,7 +2876,7 @@
         <v>147</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C142" s="1"/>
     </row>
@@ -2887,7 +2885,7 @@
         <v>148</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C143" s="1"/>
     </row>
@@ -2896,7 +2894,7 @@
         <v>149</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C144" s="1"/>
     </row>
@@ -2905,7 +2903,7 @@
         <v>150</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C145" s="1"/>
     </row>
@@ -2914,7 +2912,7 @@
         <v>151</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C146" s="1"/>
     </row>
@@ -2923,7 +2921,7 @@
         <v>152</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C147" s="1"/>
     </row>
@@ -2932,7 +2930,7 @@
         <v>153</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C148" s="1"/>
     </row>
@@ -2941,7 +2939,7 @@
         <v>154</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C149" s="1"/>
     </row>
@@ -2950,7 +2948,7 @@
         <v>155</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C150" s="1"/>
     </row>
@@ -2959,7 +2957,7 @@
         <v>156</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C151" s="1"/>
     </row>
@@ -2968,7 +2966,7 @@
         <v>157</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C152" s="1"/>
     </row>
@@ -2977,7 +2975,7 @@
         <v>158</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C153" s="1"/>
     </row>
@@ -2986,7 +2984,7 @@
         <v>159</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C154" s="1"/>
     </row>
@@ -2995,7 +2993,7 @@
         <v>160</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C155" s="1"/>
     </row>
@@ -3004,7 +3002,7 @@
         <v>161</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C156" s="1"/>
     </row>
@@ -3013,7 +3011,7 @@
         <v>162</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C157" s="1"/>
     </row>
@@ -3022,7 +3020,7 @@
         <v>163</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C158" s="1"/>
     </row>
@@ -3031,7 +3029,7 @@
         <v>164</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C159" s="1"/>
     </row>
@@ -3040,7 +3038,7 @@
         <v>165</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C160" s="1"/>
     </row>
@@ -3049,7 +3047,7 @@
         <v>166</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C161" s="1"/>
     </row>
@@ -3058,7 +3056,7 @@
         <v>167</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C162" s="1"/>
     </row>
@@ -3067,7 +3065,7 @@
         <v>168</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C163" s="1"/>
     </row>
@@ -3076,7 +3074,7 @@
         <v>169</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C164" s="1"/>
     </row>
@@ -3085,7 +3083,7 @@
         <v>170</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C165" s="1"/>
     </row>
@@ -3094,7 +3092,7 @@
         <v>171</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C166" s="1"/>
     </row>
@@ -3103,7 +3101,7 @@
         <v>172</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C167" s="1"/>
     </row>
@@ -3112,7 +3110,7 @@
         <v>173</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C168" s="1"/>
     </row>
@@ -3121,7 +3119,7 @@
         <v>174</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C169" s="1"/>
     </row>
@@ -3130,7 +3128,7 @@
         <v>175</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C170" s="1"/>
     </row>
@@ -3139,7 +3137,7 @@
         <v>176</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C171" s="1"/>
     </row>
@@ -3148,7 +3146,7 @@
         <v>177</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C172" s="1"/>
     </row>
@@ -3157,7 +3155,7 @@
         <v>178</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C173" s="1"/>
     </row>
@@ -3166,7 +3164,7 @@
         <v>179</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C174" s="1"/>
     </row>
@@ -3175,7 +3173,7 @@
         <v>180</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C175" s="1"/>
     </row>
@@ -3184,7 +3182,7 @@
         <v>181</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C176" s="1"/>
     </row>
@@ -3193,7 +3191,7 @@
         <v>182</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C177" s="1"/>
     </row>
@@ -3202,7 +3200,7 @@
         <v>183</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C178" s="1"/>
     </row>
@@ -3211,7 +3209,7 @@
         <v>184</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C179" s="1"/>
     </row>
@@ -3220,7 +3218,7 @@
         <v>185</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C180" s="1"/>
     </row>
@@ -3229,7 +3227,7 @@
         <v>186</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C181" s="1"/>
     </row>
@@ -3238,7 +3236,7 @@
         <v>187</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C182" s="1"/>
     </row>
@@ -3247,7 +3245,7 @@
         <v>188</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C183" s="1"/>
     </row>
@@ -3256,7 +3254,7 @@
         <v>189</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C184" s="1"/>
     </row>
@@ -3265,7 +3263,7 @@
         <v>190</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C185" s="1"/>
     </row>
@@ -3274,7 +3272,7 @@
         <v>191</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C186" s="1"/>
     </row>
@@ -3283,7 +3281,7 @@
         <v>192</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C187" s="1"/>
     </row>
@@ -3292,7 +3290,7 @@
         <v>193</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C188" s="1"/>
     </row>
@@ -3301,7 +3299,7 @@
         <v>194</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C189" s="1"/>
     </row>
@@ -3310,7 +3308,7 @@
         <v>195</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C190" s="1"/>
     </row>
@@ -3319,7 +3317,7 @@
         <v>196</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C191" s="1"/>
     </row>
@@ -3328,7 +3326,7 @@
         <v>197</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C192" s="1"/>
     </row>
@@ -3337,7 +3335,7 @@
         <v>198</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C193" s="1"/>
     </row>
@@ -3346,7 +3344,7 @@
         <v>199</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C194" s="1"/>
     </row>
@@ -3355,7 +3353,7 @@
         <v>200</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C195" s="1"/>
     </row>
@@ -3364,7 +3362,7 @@
         <v>201</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C196" s="1"/>
     </row>
@@ -3373,7 +3371,7 @@
         <v>202</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C197" s="1"/>
     </row>
@@ -3382,7 +3380,7 @@
         <v>203</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C198" s="1"/>
     </row>
@@ -3391,7 +3389,7 @@
         <v>204</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C199" s="1"/>
     </row>
@@ -3400,7 +3398,7 @@
         <v>205</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C200" s="1"/>
     </row>
@@ -3409,7 +3407,7 @@
         <v>206</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C201" s="1"/>
     </row>
@@ -3418,7 +3416,7 @@
         <v>207</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C202" s="1"/>
     </row>
@@ -3427,7 +3425,7 @@
         <v>208</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C203" s="1"/>
     </row>
@@ -3436,7 +3434,7 @@
         <v>209</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C204" s="1"/>
     </row>
@@ -3445,7 +3443,7 @@
         <v>210</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C205" s="1"/>
     </row>
@@ -3454,7 +3452,7 @@
         <v>211</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C206" s="1"/>
     </row>
@@ -3463,7 +3461,7 @@
         <v>212</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C207" s="1"/>
     </row>
@@ -3472,7 +3470,7 @@
         <v>213</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C208" s="1"/>
     </row>
@@ -3481,7 +3479,7 @@
         <v>214</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C209" s="1"/>
     </row>
@@ -3490,7 +3488,7 @@
         <v>215</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C210" s="1"/>
     </row>
@@ -3499,7 +3497,7 @@
         <v>216</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C211" s="1"/>
     </row>
@@ -3508,7 +3506,7 @@
         <v>217</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C212" s="1"/>
     </row>
@@ -3517,7 +3515,7 @@
         <v>218</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C213" s="1"/>
     </row>
@@ -3526,7 +3524,7 @@
         <v>219</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C214" s="1"/>
     </row>
@@ -3535,7 +3533,7 @@
         <v>220</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C215" s="1"/>
     </row>
@@ -3544,7 +3542,7 @@
         <v>221</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C216" s="1"/>
     </row>
@@ -3553,7 +3551,7 @@
         <v>222</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C217" s="1"/>
     </row>
@@ -3562,7 +3560,7 @@
         <v>223</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C218" s="1"/>
     </row>
@@ -3571,7 +3569,7 @@
         <v>224</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C219" s="1"/>
     </row>
@@ -3580,7 +3578,7 @@
         <v>225</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C220" s="1"/>
     </row>
@@ -3589,7 +3587,7 @@
         <v>226</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C221" s="1"/>
     </row>
@@ -3598,7 +3596,7 @@
         <v>227</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C222" s="1"/>
     </row>
@@ -3607,7 +3605,7 @@
         <v>228</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C223" s="1"/>
     </row>
@@ -3616,7 +3614,7 @@
         <v>229</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C224" s="1"/>
     </row>
@@ -3625,7 +3623,7 @@
         <v>230</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C225" s="1"/>
     </row>
@@ -3634,7 +3632,7 @@
         <v>231</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C226" s="1"/>
     </row>
@@ -3643,7 +3641,7 @@
         <v>232</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C227" s="1"/>
     </row>
@@ -3652,7 +3650,7 @@
         <v>233</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C228" s="1"/>
     </row>
@@ -3661,7 +3659,7 @@
         <v>234</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C229" s="1"/>
     </row>
@@ -3670,7 +3668,7 @@
         <v>235</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C230" s="1"/>
     </row>
@@ -3679,7 +3677,7 @@
         <v>236</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C231" s="1"/>
     </row>
@@ -3688,7 +3686,7 @@
         <v>237</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C232" s="1"/>
     </row>
@@ -3697,7 +3695,7 @@
         <v>238</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C233" s="1"/>
     </row>
@@ -3706,7 +3704,7 @@
         <v>239</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C234" s="1"/>
     </row>
@@ -3715,7 +3713,7 @@
         <v>240</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C235" s="1"/>
     </row>
@@ -3724,7 +3722,7 @@
         <v>241</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C236" s="1"/>
     </row>
@@ -3733,7 +3731,7 @@
         <v>242</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C237" s="1"/>
     </row>
@@ -3742,7 +3740,7 @@
         <v>243</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C238" s="1"/>
     </row>
@@ -3751,7 +3749,7 @@
         <v>244</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C239" s="1"/>
     </row>
@@ -3760,7 +3758,7 @@
         <v>245</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C240" s="1"/>
     </row>
@@ -3769,7 +3767,7 @@
         <v>246</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C241" s="1"/>
     </row>
@@ -3778,7 +3776,7 @@
         <v>247</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C242" s="1"/>
     </row>
@@ -3787,7 +3785,7 @@
         <v>248</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C243" s="1"/>
     </row>
@@ -3796,7 +3794,7 @@
         <v>249</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C244" s="1"/>
     </row>
@@ -3805,7 +3803,7 @@
         <v>250</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C245" s="1"/>
     </row>
@@ -3814,7 +3812,7 @@
         <v>251</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C246" s="1"/>
     </row>
@@ -3823,7 +3821,7 @@
         <v>252</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C247" s="1"/>
     </row>
@@ -3832,7 +3830,7 @@
         <v>253</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C248" s="1"/>
     </row>
@@ -3841,7 +3839,7 @@
         <v>254</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C249" s="1"/>
     </row>
@@ -3850,7 +3848,7 @@
         <v>255</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C250" s="1"/>
     </row>
@@ -3859,7 +3857,7 @@
         <v>256</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C251" s="1"/>
     </row>
@@ -3868,7 +3866,7 @@
         <v>257</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C252" s="1"/>
     </row>
@@ -3877,7 +3875,7 @@
         <v>258</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C253" s="1"/>
     </row>
@@ -3886,7 +3884,7 @@
         <v>259</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C254" s="1"/>
     </row>
@@ -3895,7 +3893,7 @@
         <v>260</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C255" s="1"/>
     </row>
@@ -3904,7 +3902,7 @@
         <v>261</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C256" s="1"/>
     </row>
@@ -3913,7 +3911,7 @@
         <v>262</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C257" s="1"/>
     </row>
@@ -3922,7 +3920,7 @@
         <v>263</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C258" s="1"/>
     </row>
@@ -3931,7 +3929,7 @@
         <v>264</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C259" s="1"/>
     </row>
@@ -3940,7 +3938,7 @@
         <v>265</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C260" s="1"/>
     </row>
@@ -3949,7 +3947,7 @@
         <v>266</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C261" s="1"/>
     </row>
@@ -3958,7 +3956,7 @@
         <v>267</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C262" s="1"/>
     </row>
@@ -3967,7 +3965,7 @@
         <v>268</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C263" s="1"/>
     </row>
@@ -3976,7 +3974,7 @@
         <v>269</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C264" s="1"/>
     </row>
@@ -3985,7 +3983,7 @@
         <v>270</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C265" s="1"/>
     </row>
@@ -3994,7 +3992,7 @@
         <v>271</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C266" s="1"/>
     </row>
@@ -4003,7 +4001,7 @@
         <v>272</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C267" s="1"/>
     </row>
@@ -4012,7 +4010,7 @@
         <v>273</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C268" s="1"/>
     </row>
@@ -4021,7 +4019,7 @@
         <v>274</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C269" s="1"/>
     </row>
@@ -4030,7 +4028,7 @@
         <v>275</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C270" s="1"/>
     </row>
@@ -4039,7 +4037,7 @@
         <v>276</v>
       </c>
       <c r="B271" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C271" s="1"/>
     </row>
@@ -4048,7 +4046,7 @@
         <v>277</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C272" s="1"/>
     </row>
@@ -4057,7 +4055,7 @@
         <v>278</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C273" s="1"/>
     </row>
@@ -4066,7 +4064,7 @@
         <v>279</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C274" s="1"/>
     </row>
@@ -4075,7 +4073,7 @@
         <v>280</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C275" s="1"/>
     </row>
@@ -4084,7 +4082,7 @@
         <v>281</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C276" s="1"/>
     </row>
@@ -4093,7 +4091,7 @@
         <v>282</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C277" s="1"/>
     </row>
@@ -4102,7 +4100,7 @@
         <v>283</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C278" s="1"/>
     </row>
@@ -4111,7 +4109,7 @@
         <v>284</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C279" s="1"/>
     </row>
@@ -4120,7 +4118,7 @@
         <v>285</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C280" s="1"/>
     </row>
@@ -4129,7 +4127,7 @@
         <v>286</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C281" s="1"/>
     </row>
@@ -4138,7 +4136,7 @@
         <v>287</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C282" s="1"/>
     </row>
@@ -4147,7 +4145,7 @@
         <v>288</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C283" s="1"/>
     </row>
@@ -4156,7 +4154,7 @@
         <v>289</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C284" s="1"/>
     </row>
@@ -4165,7 +4163,7 @@
         <v>290</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C285" s="1"/>
     </row>
@@ -4174,7 +4172,7 @@
         <v>291</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C286" s="1"/>
     </row>
@@ -4183,7 +4181,7 @@
         <v>292</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C287" s="1"/>
     </row>
@@ -4192,7 +4190,7 @@
         <v>293</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C288" s="1"/>
     </row>
@@ -4201,7 +4199,7 @@
         <v>294</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C289" s="1"/>
     </row>
@@ -4210,7 +4208,7 @@
         <v>295</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C290" s="1"/>
     </row>
@@ -4219,7 +4217,7 @@
         <v>296</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C291" s="1"/>
     </row>
@@ -4228,7 +4226,7 @@
         <v>297</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C292" s="1"/>
     </row>
@@ -4237,7 +4235,7 @@
         <v>298</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C293" s="1"/>
     </row>
@@ -4246,7 +4244,7 @@
         <v>299</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C294" s="1"/>
     </row>
@@ -4255,7 +4253,7 @@
         <v>300</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C295" s="1"/>
     </row>
@@ -4264,7 +4262,7 @@
         <v>301</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C296" s="1"/>
     </row>
@@ -4273,7 +4271,7 @@
         <v>302</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C297" s="1"/>
     </row>
@@ -4282,7 +4280,7 @@
         <v>303</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C298" s="1"/>
     </row>
@@ -4291,7 +4289,7 @@
         <v>304</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C299" s="1"/>
     </row>
@@ -4300,7 +4298,7 @@
         <v>305</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C300" s="1"/>
     </row>
@@ -4309,7 +4307,7 @@
         <v>306</v>
       </c>
       <c r="B301" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C301" s="1"/>
     </row>
@@ -4318,7 +4316,7 @@
         <v>307</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C302" s="1"/>
     </row>
@@ -4327,7 +4325,7 @@
         <v>308</v>
       </c>
       <c r="B303" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C303" s="1"/>
     </row>
@@ -4336,7 +4334,7 @@
         <v>309</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C304" s="1"/>
     </row>
@@ -4345,7 +4343,7 @@
         <v>310</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C305" s="1"/>
     </row>
@@ -4354,7 +4352,7 @@
         <v>311</v>
       </c>
       <c r="B306" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C306" s="1"/>
     </row>
@@ -4363,7 +4361,7 @@
         <v>312</v>
       </c>
       <c r="B307" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C307" s="1"/>
     </row>
@@ -4372,7 +4370,7 @@
         <v>313</v>
       </c>
       <c r="B308" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C308" s="1"/>
     </row>
@@ -4381,7 +4379,7 @@
         <v>314</v>
       </c>
       <c r="B309" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C309" s="1"/>
     </row>
@@ -4390,7 +4388,7 @@
         <v>315</v>
       </c>
       <c r="B310" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C310" s="1"/>
     </row>
@@ -4399,7 +4397,7 @@
         <v>316</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C311" s="1"/>
     </row>
@@ -4408,7 +4406,7 @@
         <v>317</v>
       </c>
       <c r="B312" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C312" s="1"/>
     </row>
@@ -4417,7 +4415,7 @@
         <v>318</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C313" s="1"/>
     </row>
@@ -4426,7 +4424,7 @@
         <v>319</v>
       </c>
       <c r="B314" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C314" s="1"/>
     </row>
@@ -4435,7 +4433,7 @@
         <v>320</v>
       </c>
       <c r="B315" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C315" s="1"/>
     </row>
@@ -4444,7 +4442,7 @@
         <v>321</v>
       </c>
       <c r="B316" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C316" s="1"/>
     </row>
@@ -4453,7 +4451,7 @@
         <v>322</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C317" s="1"/>
     </row>
@@ -4462,7 +4460,7 @@
         <v>323</v>
       </c>
       <c r="B318" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C318" s="1"/>
     </row>
@@ -4471,7 +4469,7 @@
         <v>324</v>
       </c>
       <c r="B319" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C319" s="1"/>
     </row>
@@ -4480,7 +4478,7 @@
         <v>325</v>
       </c>
       <c r="B320" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C320" s="1"/>
     </row>
@@ -4489,7 +4487,7 @@
         <v>326</v>
       </c>
       <c r="B321" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C321" s="1"/>
     </row>
@@ -4498,7 +4496,7 @@
         <v>327</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C322" s="1"/>
     </row>
@@ -4507,7 +4505,7 @@
         <v>328</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C323" s="1"/>
     </row>
@@ -4516,7 +4514,7 @@
         <v>329</v>
       </c>
       <c r="B324" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C324" s="1"/>
     </row>
@@ -4525,7 +4523,7 @@
         <v>330</v>
       </c>
       <c r="B325" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C325" s="1"/>
     </row>
@@ -4534,7 +4532,7 @@
         <v>331</v>
       </c>
       <c r="B326" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C326" s="1"/>
     </row>
@@ -4543,7 +4541,7 @@
         <v>332</v>
       </c>
       <c r="B327" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C327" s="1"/>
     </row>
@@ -4552,7 +4550,7 @@
         <v>333</v>
       </c>
       <c r="B328" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C328" s="1"/>
     </row>
@@ -4561,7 +4559,7 @@
         <v>334</v>
       </c>
       <c r="B329" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C329" s="1"/>
     </row>
@@ -4570,7 +4568,7 @@
         <v>335</v>
       </c>
       <c r="B330" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C330" s="1"/>
     </row>
@@ -4579,7 +4577,7 @@
         <v>336</v>
       </c>
       <c r="B331" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C331" s="1"/>
     </row>
@@ -4588,7 +4586,7 @@
         <v>337</v>
       </c>
       <c r="B332" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C332" s="1"/>
     </row>
@@ -4597,7 +4595,7 @@
         <v>338</v>
       </c>
       <c r="B333" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C333" s="1"/>
     </row>
@@ -4606,7 +4604,7 @@
         <v>339</v>
       </c>
       <c r="B334" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C334" s="1"/>
     </row>
@@ -4615,7 +4613,7 @@
         <v>340</v>
       </c>
       <c r="B335" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C335" s="1"/>
     </row>
@@ -4624,7 +4622,7 @@
         <v>341</v>
       </c>
       <c r="B336" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C336" s="1"/>
     </row>
@@ -4633,7 +4631,7 @@
         <v>342</v>
       </c>
       <c r="B337" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C337" s="1"/>
     </row>
@@ -4642,7 +4640,7 @@
         <v>343</v>
       </c>
       <c r="B338" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C338" s="1"/>
     </row>
@@ -4651,7 +4649,7 @@
         <v>344</v>
       </c>
       <c r="B339" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C339" s="1"/>
     </row>
@@ -4660,7 +4658,7 @@
         <v>345</v>
       </c>
       <c r="B340" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C340" s="1"/>
     </row>
@@ -4669,7 +4667,7 @@
         <v>346</v>
       </c>
       <c r="B341" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C341" s="1"/>
     </row>
@@ -4678,7 +4676,7 @@
         <v>347</v>
       </c>
       <c r="B342" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C342" s="1"/>
     </row>
@@ -4687,7 +4685,7 @@
         <v>348</v>
       </c>
       <c r="B343" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C343" s="1"/>
     </row>
@@ -4696,7 +4694,7 @@
         <v>349</v>
       </c>
       <c r="B344" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C344" s="1"/>
     </row>
@@ -4705,7 +4703,7 @@
         <v>350</v>
       </c>
       <c r="B345" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C345" s="1"/>
     </row>
@@ -4714,7 +4712,7 @@
         <v>351</v>
       </c>
       <c r="B346" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C346" s="1"/>
     </row>
@@ -4723,7 +4721,7 @@
         <v>352</v>
       </c>
       <c r="B347" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C347" s="1"/>
     </row>
@@ -4732,7 +4730,7 @@
         <v>353</v>
       </c>
       <c r="B348" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C348" s="1"/>
     </row>
@@ -4741,7 +4739,7 @@
         <v>354</v>
       </c>
       <c r="B349" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C349" s="1"/>
     </row>
@@ -4750,7 +4748,7 @@
         <v>355</v>
       </c>
       <c r="B350" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C350" s="1"/>
     </row>
@@ -4759,7 +4757,7 @@
         <v>356</v>
       </c>
       <c r="B351" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C351" s="1"/>
     </row>
@@ -4768,7 +4766,7 @@
         <v>357</v>
       </c>
       <c r="B352" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C352" s="1"/>
     </row>
@@ -4777,7 +4775,7 @@
         <v>358</v>
       </c>
       <c r="B353" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C353" s="1"/>
     </row>
@@ -4786,7 +4784,7 @@
         <v>359</v>
       </c>
       <c r="B354" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C354" s="1"/>
     </row>
@@ -4795,7 +4793,7 @@
         <v>360</v>
       </c>
       <c r="B355" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C355" s="1"/>
     </row>
@@ -4804,7 +4802,7 @@
         <v>361</v>
       </c>
       <c r="B356" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C356" s="1"/>
     </row>
@@ -4813,7 +4811,7 @@
         <v>362</v>
       </c>
       <c r="B357" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C357" s="1"/>
     </row>
@@ -4822,7 +4820,7 @@
         <v>363</v>
       </c>
       <c r="B358" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C358" s="1"/>
     </row>
@@ -4831,7 +4829,7 @@
         <v>364</v>
       </c>
       <c r="B359" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C359" s="1"/>
     </row>
@@ -4840,7 +4838,7 @@
         <v>365</v>
       </c>
       <c r="B360" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C360" s="1"/>
     </row>
@@ -4849,7 +4847,7 @@
         <v>366</v>
       </c>
       <c r="B361" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C361" s="1"/>
     </row>
@@ -4858,7 +4856,7 @@
         <v>367</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C362" s="1"/>
     </row>
@@ -4867,7 +4865,7 @@
         <v>368</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C363" s="1"/>
     </row>
@@ -4876,7 +4874,7 @@
         <v>369</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C364" s="1"/>
     </row>
@@ -4885,7 +4883,7 @@
         <v>370</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C365" s="1"/>
     </row>
@@ -4894,7 +4892,7 @@
         <v>371</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C366" s="1"/>
     </row>
@@ -4903,7 +4901,7 @@
         <v>372</v>
       </c>
       <c r="B367" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C367" s="1"/>
     </row>
@@ -4912,7 +4910,7 @@
         <v>373</v>
       </c>
       <c r="B368" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C368" s="1"/>
     </row>
@@ -4921,7 +4919,7 @@
         <v>374</v>
       </c>
       <c r="B369" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C369" s="1"/>
     </row>
@@ -4930,7 +4928,7 @@
         <v>375</v>
       </c>
       <c r="B370" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C370" s="1"/>
     </row>
@@ -4939,7 +4937,7 @@
         <v>376</v>
       </c>
       <c r="B371" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C371" s="1"/>
     </row>
@@ -4948,7 +4946,7 @@
         <v>377</v>
       </c>
       <c r="B372" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C372" s="1"/>
     </row>
@@ -4957,7 +4955,7 @@
         <v>378</v>
       </c>
       <c r="B373" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C373" s="1"/>
     </row>
@@ -4966,7 +4964,7 @@
         <v>379</v>
       </c>
       <c r="B374" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C374" s="1"/>
     </row>
@@ -4975,7 +4973,7 @@
         <v>380</v>
       </c>
       <c r="B375" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C375" s="1"/>
     </row>
@@ -4984,7 +4982,7 @@
         <v>381</v>
       </c>
       <c r="B376" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C376" s="1"/>
     </row>
@@ -4993,7 +4991,7 @@
         <v>382</v>
       </c>
       <c r="B377" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C377" s="1"/>
     </row>
@@ -5002,7 +5000,7 @@
         <v>383</v>
       </c>
       <c r="B378" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C378" s="1"/>
     </row>
@@ -5011,7 +5009,7 @@
         <v>384</v>
       </c>
       <c r="B379" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C379" s="1"/>
     </row>
@@ -5020,7 +5018,7 @@
         <v>385</v>
       </c>
       <c r="B380" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C380" s="1"/>
     </row>
@@ -5029,7 +5027,7 @@
         <v>386</v>
       </c>
       <c r="B381" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C381" s="1"/>
     </row>
@@ -5038,7 +5036,7 @@
         <v>387</v>
       </c>
       <c r="B382" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C382" s="1"/>
     </row>
@@ -5047,7 +5045,7 @@
         <v>388</v>
       </c>
       <c r="B383" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C383" s="1"/>
     </row>
@@ -5056,7 +5054,7 @@
         <v>389</v>
       </c>
       <c r="B384" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C384" s="1"/>
     </row>
@@ -5065,7 +5063,7 @@
         <v>390</v>
       </c>
       <c r="B385" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C385" s="1"/>
     </row>
@@ -5074,7 +5072,7 @@
         <v>391</v>
       </c>
       <c r="B386" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C386" s="1"/>
     </row>
@@ -5083,7 +5081,7 @@
         <v>392</v>
       </c>
       <c r="B387" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C387" s="1"/>
     </row>
@@ -5092,7 +5090,7 @@
         <v>393</v>
       </c>
       <c r="B388" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C388" s="1"/>
     </row>
@@ -5101,7 +5099,7 @@
         <v>394</v>
       </c>
       <c r="B389" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C389" s="1"/>
     </row>
@@ -5110,7 +5108,7 @@
         <v>395</v>
       </c>
       <c r="B390" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C390" s="1"/>
     </row>
@@ -5119,7 +5117,7 @@
         <v>396</v>
       </c>
       <c r="B391" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C391" s="1"/>
     </row>
@@ -5128,7 +5126,7 @@
         <v>397</v>
       </c>
       <c r="B392" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C392" s="1"/>
     </row>
@@ -5137,7 +5135,7 @@
         <v>398</v>
       </c>
       <c r="B393" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C393" s="1"/>
     </row>
@@ -5146,7 +5144,7 @@
         <v>399</v>
       </c>
       <c r="B394" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C394" s="1"/>
     </row>
@@ -5155,7 +5153,7 @@
         <v>400</v>
       </c>
       <c r="B395" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C395" s="1"/>
     </row>
@@ -5164,7 +5162,7 @@
         <v>401</v>
       </c>
       <c r="B396" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C396" s="1"/>
     </row>
@@ -5173,7 +5171,7 @@
         <v>402</v>
       </c>
       <c r="B397" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C397" s="1"/>
     </row>
@@ -5182,7 +5180,7 @@
         <v>403</v>
       </c>
       <c r="B398" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C398" s="1"/>
     </row>
@@ -5191,7 +5189,7 @@
         <v>404</v>
       </c>
       <c r="B399" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C399" s="1"/>
     </row>
@@ -5200,7 +5198,7 @@
         <v>405</v>
       </c>
       <c r="B400" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C400" s="1"/>
     </row>
@@ -5209,6 +5207,6 @@
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Debug saveFile - does not work on Heroku
</commit_message>
<xml_diff>
--- a/SeminarDatasheet.xlsx
+++ b/SeminarDatasheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Stuff\Development\Python\excel-bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E0FBE6-4381-4997-825C-4AF6A4861ADC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A20EBD8-5690-44A2-ACED-D68E6F08482B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8445" yWindow="3000" windowWidth="14400" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1587,7 +1587,7 @@
   <dimension ref="A1:D400"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1596,8 +1596,8 @@
     <col min="2" max="2" width="6" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="9.140625" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="5" max="6" width="9.140625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Edited messages as requested
</commit_message>
<xml_diff>
--- a/SeminarDatasheet.xlsx
+++ b/SeminarDatasheet.xlsx
@@ -396,7 +396,11 @@
           <t>A</t>
         </is>
       </c>
-      <c r="C2" s="1" t="inlineStr"/>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">

</xml_diff>